<commit_message>
zss-577/zss 606 , release note and re-add testcase for
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/577-chart.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/577-chart.xlsx
@@ -223,6 +223,97 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$B$1,Sheet1!$B$3)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$A$1,Sheet1!$A$3)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -250,6 +341,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1514475</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -548,7 +671,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>